<commit_message>
bound in solve, and read excel sheets with formulas
</commit_message>
<xml_diff>
--- a/dataUncert/testData/data1.xlsx
+++ b/dataUncert/testData/data1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\ymerdkdc01\folder redirections\DJAVE\My Documents\GitHub\dataUncert\dataUncert\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DJAVE\AppData\Local\Programs\Python\Python311\Lib\site-packages\dataUncert\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9AFC18D-06B0-42A1-8B5B-8B59ED5D08F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{888DC197-475C-4CA8-AA53-AB9C64BB4CF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{F5F6BAB0-B9A3-4FB8-B84A-62DE77F5D537}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F5F6BAB0-B9A3-4FB8-B84A-62DE77F5D537}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -401,12 +401,12 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A4" sqref="A4:A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -414,7 +414,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -422,7 +422,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -430,32 +430,36 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f>A3+1</f>
         <v>2</v>
       </c>
       <c r="B4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" ref="A5:A7" si="0">A4+1</f>
         <v>3</v>
       </c>
       <c r="B5">
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B6">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B7">

</xml_diff>